<commit_message>
Activities completed: Data restrictions placed in four columns, including those from the examples in the lessons (no_members and respondent_wall_type) and my own (rooms and months_lack_food)
</commit_message>
<xml_diff>
--- a/DataCarpentry_QualityAssuranceActivity.xlsx
+++ b/DataCarpentry_QualityAssuranceActivity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emily/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emily/Hunt-Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C74670-6F1B-D740-AE44-70C8BBACF7AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB375C56-88F6-DA4D-BBE2-B3B6BE6D1C76}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="460" windowWidth="25440" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="25600" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCarpentry_Quality" sheetId="1" r:id="rId1"/>
@@ -1781,11 +1781,13 @@
   <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" customWidth="1"/>
     <col min="13" max="13" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7598,6 +7600,22 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data Is Invalid" error="You entered a whole number that was not between 1 and 30." promptTitle="Invalid Data" prompt="Number of household members must be a whole number between 1 and 30." sqref="D1:D1048576" xr:uid="{962BB15D-E76E-834C-BCC2-D0A0FC6B0DC5}">
+      <formula1>1</formula1>
+      <formula2>30</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data Is Invalid" error="You entered a whole number that was not between 1 and 10." promptTitle="Invalid Data" prompt="The number of rooms must be a whole number between 1 and 10." sqref="G1:G1048576" xr:uid="{4571A15B-14E8-3D4D-90B5-779971862059}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data is Invalid" error="You entered a wall type that was not grass, muddaub, burntbricks, sunbricks or cement." promptTitle="Invalid Data" prompt="Wall type must be either grass, muddaub, burntbricks, sunbricks or cement." sqref="F1:F1048576" xr:uid="{1B5E7D78-A8A9-0D47-B076-0497840AB974}">
+      <formula1>"grass, muddaub, burntbricks, sunbricks, cement"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data is Invalid" error="You entered a month that was not Jan, Feb, Mar, Apr, May, June, July, Aug, Sept, Oct, Nov or Dec." promptTitle="Invalid Data" prompt="The month abbreviation must be Jan, Feb, Mar, Apr, May, June, July, Aug, Sept, Oct, Nov or Dec." sqref="M1:M1048576" xr:uid="{AA8ECD24-4A10-104B-850F-F29CC0F90EDD}">
+      <formula1>"Jan, Feb, Mar, Apr, May, June, July, Aug, Sept, Oct, Nov, Dec"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data validation rule removed from months_lack_food column, and one added to affect_conflict column.
</commit_message>
<xml_diff>
--- a/DataCarpentry_QualityAssuranceActivity.xlsx
+++ b/DataCarpentry_QualityAssuranceActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emily/Hunt-Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB375C56-88F6-DA4D-BBE2-B3B6BE6D1C76}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E43804-AD33-E84B-9E5C-CFE0329CC620}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="25600" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="460" windowWidth="25600" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCarpentry_Quality" sheetId="1" r:id="rId1"/>
@@ -1781,7 +1781,7 @@
   <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7612,8 +7612,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data is Invalid" error="You entered a wall type that was not grass, muddaub, burntbricks, sunbricks or cement." promptTitle="Invalid Data" prompt="Wall type must be either grass, muddaub, burntbricks, sunbricks or cement." sqref="F1:F1048576" xr:uid="{1B5E7D78-A8A9-0D47-B076-0497840AB974}">
       <formula1>"grass, muddaub, burntbricks, sunbricks, cement"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data is Invalid" error="You entered a month that was not Jan, Feb, Mar, Apr, May, June, July, Aug, Sept, Oct, Nov or Dec." promptTitle="Invalid Data" prompt="The month abbreviation must be Jan, Feb, Mar, Apr, May, June, July, Aug, Sept, Oct, Nov or Dec." sqref="M1:M1048576" xr:uid="{AA8ECD24-4A10-104B-850F-F29CC0F90EDD}">
-      <formula1>"Jan, Feb, Mar, Apr, May, June, July, Aug, Sept, Oct, Nov, Dec"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This Data Is Invalid" error="You entered an effect that was not never, once, more_once, frequently or NULL." promptTitle="Invalid Data" prompt="Conflict effect must be either never, once, more_once, frequently or NULL." sqref="I1:I1048576" xr:uid="{7EFFC432-7060-9A4D-BDDF-B8F8DEE9DA81}">
+      <formula1>"never, once, more_once, frequently, NULL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>